<commit_message>
add dataset -- AG News
</commit_message>
<xml_diff>
--- a/dataset/公开数据集.xlsx
+++ b/dataset/公开数据集.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="数据集汇总" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="可用资源汇总" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="12 AG-news" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="163">
   <si>
     <t>相关论文列表</t>
   </si>
@@ -29,6 +30,16 @@
     <t>模型</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Nal Kalchbrenner</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -37,7 +48,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Nal Kalchbrenner，</t>
+      <t>，</t>
     </r>
     <r>
       <rPr>
@@ -355,11 +366,21 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>movie reviews</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>movie reviews，</t>
+      <t>，</t>
     </r>
     <r>
       <rPr>
@@ -389,11 +410,21 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>electronics product reviews</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>electronics product reviews，</t>
+      <t>，</t>
     </r>
     <r>
       <rPr>
@@ -459,6 +490,12 @@
     <t>Xuan-Hieu Phan, et al.2008. Learning to classify short and sparse text &amp; web with hidden topicsfrom large-scale data collections.</t>
   </si>
   <si>
+    <t>AG’s News</t>
+  </si>
+  <si>
+    <t>AG is a collection of more than 1 million news articles</t>
+  </si>
+  <si>
     <t>统计的是正确率</t>
   </si>
   <si>
@@ -468,6 +505,16 @@
     <t>模型\数据集</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Kalchbrenner</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -476,7 +523,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Kalchbrenner，</t>
+      <t>，</t>
     </r>
     <r>
       <rPr>
@@ -515,11 +562,21 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Paragraph-Vec(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Paragraph-Vec(数据来自</t>
+      <t>数据来自</t>
     </r>
     <r>
       <rPr>
@@ -598,6 +655,162 @@
   <si>
     <t>情感词库</t>
   </si>
+  <si>
+    <t>下载地址</t>
+  </si>
+  <si>
+    <t>https://github.com/zhangxiangxiao/Crepe</t>
+  </si>
+  <si>
+    <t>Xiang Zhang, et al. Character-level convolutional networks for text classification. NIPS 2015</t>
+  </si>
+  <si>
+    <t>Task Type</t>
+  </si>
+  <si>
+    <t>Topic categories.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>AG NEWs is a collection of more than 1 million news articles</t>
+  </si>
+  <si>
+    <t>类别数</t>
+  </si>
+  <si>
+    <t>类别名</t>
+  </si>
+  <si>
+    <t>World,   Sports,    Business,  Sci/Tech</t>
+  </si>
+  <si>
+    <t>句子长度</t>
+  </si>
+  <si>
+    <t>字典数</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>最长 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t>= 191 , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>最短 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t>= 3 ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>平均 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>= 34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>最长 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t>= 148 , </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>最短 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+      </rPr>
+      <t>= 6 ,  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>平均 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>= 33</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -606,7 +819,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -713,6 +926,19 @@
       <name val="宋体"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -900,7 +1126,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="113">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -921,42 +1147,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -993,16 +1223,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1065,7 +1299,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1105,10 +1339,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1137,7 +1367,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1307,6 +1537,46 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1387,29 +1657,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:60"/>
+  <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="95.7651821862348"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="54.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5465587044534"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.4534412955466"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="104.704453441296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="59.2955465587045"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.0080971659919"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.7935222672065"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.0445344129555"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6599190283401"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6963562753036"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.834008097166"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,16 +2016,16 @@
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="14" t="s">
         <v>57</v>
       </c>
       <c r="J17" s="0"/>
@@ -1764,67 +2034,67 @@
       <c r="A18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="18" t="s">
+      <c r="L18" s="19" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="15" t="n">
+      <c r="D19" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="15" t="n">
+      <c r="F19" s="16" t="n">
         <v>11855</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="15" t="n">
+      <c r="H19" s="16" t="n">
         <v>8544</v>
       </c>
       <c r="I19" s="0"/>
-      <c r="J19" s="15" t="n">
+      <c r="J19" s="16" t="n">
         <v>1101</v>
       </c>
-      <c r="K19" s="15" t="n">
+      <c r="K19" s="16" t="n">
         <v>2210</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="16" t="s">
         <v>70</v>
       </c>
       <c r="M19" s="1"/>
@@ -1833,86 +2103,86 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="15" t="n">
+      <c r="D20" s="16" t="n">
         <v>2</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="15" t="n">
+      <c r="F20" s="16" t="n">
         <v>9613</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="15" t="n">
+      <c r="H20" s="16" t="n">
         <v>6920</v>
       </c>
       <c r="I20" s="0"/>
-      <c r="J20" s="15" t="n">
+      <c r="J20" s="16" t="n">
         <v>872</v>
       </c>
-      <c r="K20" s="15" t="n">
+      <c r="K20" s="16" t="n">
         <v>1821</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="M20" s="15"/>
+      <c r="M20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="61.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
+      <c r="A21" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D21" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="F21" s="16" t="n">
         <v>5952</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="15" t="n">
+      <c r="H21" s="16" t="n">
         <v>5452</v>
       </c>
       <c r="I21" s="0"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15" t="n">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16" t="n">
         <v>500</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+      <c r="A22" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="16" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -1920,16 +2190,16 @@
       </c>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="16" t="s">
         <v>83</v>
       </c>
       <c r="I22" s="0"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15" t="n">
+      <c r="J22" s="16"/>
+      <c r="K22" s="16" t="n">
         <v>400</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15" t="n">
+      <c r="L22" s="16"/>
+      <c r="M22" s="16" t="n">
         <v>76643</v>
       </c>
       <c r="N22" s="0" t="s">
@@ -1940,10 +2210,10 @@
       <c r="A23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D23" s="1" t="n">
@@ -1952,10 +2222,10 @@
       <c r="E23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="17" t="s">
         <v>89</v>
       </c>
       <c r="H23" s="0"/>
@@ -1971,10 +2241,10 @@
       <c r="A24" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D24" s="1" t="n">
@@ -2000,10 +2270,10 @@
       <c r="A25" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="16" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="1" t="n">
@@ -2026,13 +2296,13 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="n">
+      <c r="A26" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D26" s="1" t="n">
@@ -2058,13 +2328,13 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="n">
+      <c r="A27" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D27" s="1" t="n">
@@ -2091,10 +2361,10 @@
       <c r="B28" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="17" t="s">
         <v>105</v>
       </c>
       <c r="E28" s="9" t="s">
@@ -2118,7 +2388,7 @@
       <c r="B29" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="26" t="s">
         <v>109</v>
       </c>
       <c r="D29" s="1" t="n">
@@ -2138,14 +2408,14 @@
         <v>49838</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="n">
         <v>11</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="26" t="s">
         <v>111</v>
       </c>
       <c r="D30" s="0"/>
@@ -2165,10 +2435,18 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="0"/>
+      <c r="A31" s="27" t="n">
+        <v>12</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="E31" s="0"/>
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
@@ -2177,7 +2455,7 @@
       <c r="J31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="0"/>
@@ -2188,738 +2466,798 @@
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
     </row>
-    <row r="33" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-    </row>
-    <row r="34" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-    </row>
-    <row r="35" s="39" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="34" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="28"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="28"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="28"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="28"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+      <c r="J37" s="0"/>
+    </row>
+    <row r="38" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+    </row>
+    <row r="39" s="35" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36" t="s">
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+    </row>
+    <row r="40" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D40" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="37" t="s">
+      <c r="E40" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F40" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G40" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="H35" s="36" t="s">
+      <c r="H40" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I35" s="36" t="s">
+      <c r="I40" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="J35" s="36" t="s">
+      <c r="J40" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="K35" s="36" t="s">
+      <c r="K40" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="L35" s="38" t="s">
+      <c r="L40" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="M35" s="38" t="s">
+      <c r="M40" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="N35" s="38" t="s">
+      <c r="N40" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="O35" s="38" t="s">
+      <c r="O40" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="AMJ35" s="40"/>
-    </row>
-    <row r="36" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44" t="n">
+      <c r="AMJ40" s="42"/>
+    </row>
+    <row r="41" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="45"/>
+      <c r="D41" s="46" t="n">
         <v>48.5</v>
       </c>
-      <c r="E36" s="44" t="n">
+      <c r="E41" s="46" t="n">
         <v>86.8</v>
       </c>
-      <c r="F36" s="44" t="n">
+      <c r="F41" s="46" t="n">
         <v>93</v>
       </c>
-      <c r="G36" s="44" t="n">
+      <c r="G41" s="46" t="n">
         <v>87.4</v>
       </c>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="41"/>
-      <c r="B37" s="47" t="s">
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="43"/>
+      <c r="B42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49" t="n">
+      <c r="C42" s="50"/>
+      <c r="D42" s="51" t="n">
         <v>37.4</v>
       </c>
-      <c r="E37" s="49" t="n">
+      <c r="E42" s="51" t="n">
         <v>77.1</v>
       </c>
-      <c r="F37" s="49" t="n">
+      <c r="F42" s="51" t="n">
         <v>84.4</v>
       </c>
-      <c r="G37" s="49" t="n">
+      <c r="G42" s="51" t="n">
         <v>78.8</v>
       </c>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="50"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="41"/>
-      <c r="B38" s="47" t="s">
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="43"/>
+      <c r="B43" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49" t="n">
+      <c r="C43" s="50"/>
+      <c r="D43" s="51" t="n">
         <v>42.4</v>
       </c>
-      <c r="E38" s="49" t="n">
+      <c r="E43" s="51" t="n">
         <v>80.5</v>
       </c>
-      <c r="F38" s="49" t="n">
+      <c r="F43" s="51" t="n">
         <v>88.2</v>
       </c>
-      <c r="G38" s="49" t="n">
+      <c r="G43" s="51" t="n">
         <v>80.9</v>
       </c>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-    </row>
-    <row r="39" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="C39" s="53" t="n">
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+    </row>
+    <row r="44" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="54" t="n">
         <v>76.1</v>
       </c>
-      <c r="D39" s="53" t="n">
+      <c r="D44" s="54" t="n">
         <v>45</v>
       </c>
-      <c r="E39" s="53" t="n">
+      <c r="E44" s="54" t="n">
         <v>82.7</v>
       </c>
-      <c r="F39" s="43" t="n">
+      <c r="F44" s="45" t="n">
         <v>91.2</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43" t="n">
+      <c r="G44" s="45"/>
+      <c r="H44" s="45" t="n">
         <v>89.6</v>
       </c>
-      <c r="I39" s="43" t="n">
+      <c r="I44" s="45" t="n">
         <v>79.8</v>
       </c>
-      <c r="J39" s="43" t="n">
+      <c r="J44" s="45" t="n">
         <v>83.4</v>
       </c>
-      <c r="K39" s="43"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="51"/>
-      <c r="B40" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="49" t="n">
+      <c r="K44" s="45"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="47"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="43"/>
+      <c r="B45" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="51" t="n">
         <v>81</v>
       </c>
-      <c r="D40" s="49" t="n">
+      <c r="D45" s="51" t="n">
         <v>45.5</v>
       </c>
-      <c r="E40" s="49" t="n">
+      <c r="E45" s="51" t="n">
         <v>86.8</v>
       </c>
-      <c r="F40" s="48" t="n">
+      <c r="F45" s="50" t="n">
         <v>92.8</v>
       </c>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48" t="n">
+      <c r="G45" s="50"/>
+      <c r="H45" s="50" t="n">
         <v>93</v>
       </c>
-      <c r="I40" s="48" t="n">
+      <c r="I45" s="50" t="n">
         <v>84.7</v>
       </c>
-      <c r="J40" s="55" t="n">
+      <c r="J45" s="56" t="n">
         <v>89.6</v>
       </c>
-      <c r="K40" s="55"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="51"/>
-      <c r="B41" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" s="56" t="n">
+      <c r="K45" s="56"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="43"/>
+      <c r="B46" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="57" t="n">
         <v>81.5</v>
       </c>
-      <c r="D41" s="49" t="n">
+      <c r="D46" s="51" t="n">
         <v>48</v>
       </c>
-      <c r="E41" s="49" t="n">
+      <c r="E46" s="51" t="n">
         <v>87.2</v>
       </c>
-      <c r="F41" s="48" t="n">
+      <c r="F46" s="50" t="n">
         <v>93.6</v>
       </c>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48" t="n">
+      <c r="G46" s="50"/>
+      <c r="H46" s="50" t="n">
         <v>93.4</v>
       </c>
-      <c r="I41" s="48" t="n">
+      <c r="I46" s="50" t="n">
         <v>84.3</v>
       </c>
-      <c r="J41" s="48" t="n">
+      <c r="J46" s="50" t="n">
         <v>89.5</v>
       </c>
-      <c r="K41" s="48"/>
-      <c r="L41" s="50"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="50"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="51"/>
-      <c r="B42" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="49" t="n">
+      <c r="K46" s="50"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="43"/>
+      <c r="B47" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="51" t="n">
         <v>81.1</v>
       </c>
-      <c r="D42" s="48" t="n">
+      <c r="D47" s="50" t="n">
         <v>47.4</v>
       </c>
-      <c r="E42" s="57" t="n">
+      <c r="E47" s="58" t="n">
         <v>88.1</v>
       </c>
-      <c r="F42" s="48" t="n">
+      <c r="F47" s="50" t="n">
         <v>92.2</v>
       </c>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48" t="n">
+      <c r="G47" s="50"/>
+      <c r="H47" s="50" t="n">
         <v>93.2</v>
       </c>
-      <c r="I42" s="55" t="n">
+      <c r="I47" s="56" t="n">
         <v>85</v>
       </c>
-      <c r="J42" s="48" t="n">
+      <c r="J47" s="50" t="n">
         <v>89.4</v>
       </c>
-      <c r="K42" s="48"/>
-      <c r="L42" s="50"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-    </row>
-    <row r="43" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="60" t="n">
+      <c r="K47" s="50"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+    </row>
+    <row r="48" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="45"/>
+      <c r="D48" s="61" t="n">
         <v>48.7</v>
       </c>
-      <c r="E43" s="43" t="n">
+      <c r="E48" s="45" t="n">
         <v>87.8</v>
       </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="45"/>
-      <c r="AMJ43" s="61"/>
-    </row>
-    <row r="44" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="65" t="n">
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="AMJ48" s="62"/>
+    </row>
+    <row r="49" s="67" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="66" t="n">
         <v>95</v>
       </c>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="64"/>
-      <c r="N44" s="64"/>
-      <c r="O44" s="64"/>
-      <c r="AMJ44" s="67"/>
-    </row>
-    <row r="45" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="62" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="68" t="n">
+      <c r="G49" s="65"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="65"/>
+      <c r="K49" s="65"/>
+      <c r="L49" s="65"/>
+      <c r="M49" s="65"/>
+      <c r="N49" s="65"/>
+      <c r="O49" s="65"/>
+      <c r="AMJ49" s="68"/>
+    </row>
+    <row r="50" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="69" t="n">
         <v>79</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="68" t="n">
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="69" t="n">
         <v>93.6</v>
       </c>
-      <c r="I45" s="68" t="n">
+      <c r="I50" s="69" t="n">
         <v>80</v>
       </c>
-      <c r="J45" s="68" t="n">
+      <c r="J50" s="69" t="n">
         <v>86.3</v>
       </c>
-      <c r="K45" s="68"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="64"/>
-      <c r="N45" s="64"/>
-      <c r="O45" s="64"/>
-      <c r="AMJ45" s="67"/>
-    </row>
-    <row r="46" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="62" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="C46" s="68" t="n">
+      <c r="K50" s="69"/>
+      <c r="L50" s="65"/>
+      <c r="M50" s="65"/>
+      <c r="N50" s="65"/>
+      <c r="O50" s="65"/>
+      <c r="AMJ50" s="68"/>
+    </row>
+    <row r="51" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="69" t="n">
         <v>79.1</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="55" t="n">
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="65"/>
+      <c r="H51" s="56" t="n">
         <v>93.6</v>
       </c>
-      <c r="I46" s="68" t="n">
+      <c r="I51" s="69" t="n">
         <v>81.9</v>
       </c>
-      <c r="J46" s="68" t="n">
+      <c r="J51" s="69" t="n">
         <v>86.3</v>
       </c>
-      <c r="K46" s="68"/>
-      <c r="L46" s="68"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="64"/>
-      <c r="O46" s="64"/>
-      <c r="AMJ46" s="67"/>
-    </row>
-    <row r="47" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="70" t="s">
+      <c r="K51" s="69"/>
+      <c r="L51" s="69"/>
+      <c r="M51" s="69"/>
+      <c r="N51" s="65"/>
+      <c r="O51" s="65"/>
+      <c r="AMJ51" s="68"/>
+    </row>
+    <row r="52" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="71" t="s">
+      <c r="B52" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43" t="n">
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45" t="n">
         <v>8.66</v>
       </c>
-      <c r="M47" s="43" t="n">
+      <c r="M52" s="45" t="n">
         <v>8.39</v>
       </c>
-      <c r="N47" s="0"/>
-      <c r="O47" s="43" t="n">
+      <c r="N52" s="0"/>
+      <c r="O52" s="45" t="n">
         <v>9.33</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="70"/>
-      <c r="B48" s="72" t="s">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="71"/>
+      <c r="B53" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48" t="n">
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50" t="n">
         <v>8.39</v>
       </c>
-      <c r="M48" s="48" t="n">
+      <c r="M53" s="50" t="n">
         <v>7.64</v>
       </c>
-      <c r="N48" s="50"/>
-      <c r="O48" s="48" t="n">
+      <c r="N53" s="52"/>
+      <c r="O53" s="50" t="n">
         <v>9.96</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="70"/>
-      <c r="B49" s="72" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="71"/>
+      <c r="B54" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48" t="n">
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="50"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="50" t="n">
         <v>8.04</v>
       </c>
-      <c r="M49" s="48" t="n">
+      <c r="M54" s="50" t="n">
         <v>7.48</v>
       </c>
-      <c r="N49" s="50"/>
-      <c r="O49" s="50"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="70"/>
-      <c r="B50" s="72" t="s">
+      <c r="N54" s="52"/>
+      <c r="O54" s="52"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="71"/>
+      <c r="B55" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="73"/>
-      <c r="L50" s="74" t="n">
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="74"/>
+      <c r="L55" s="75" t="n">
         <v>7.67</v>
       </c>
-      <c r="M50" s="74" t="n">
+      <c r="M55" s="75" t="n">
         <v>7.14</v>
       </c>
-      <c r="N50" s="75"/>
-      <c r="O50" s="75"/>
-    </row>
-    <row r="51" s="46" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="76" t="s">
+      <c r="N55" s="76"/>
+      <c r="O55" s="76"/>
+    </row>
+    <row r="56" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="77" t="s">
+      <c r="B56" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="78"/>
-      <c r="D51" s="78"/>
-      <c r="E51" s="78"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="78"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
-      <c r="K51" s="78"/>
-      <c r="L51" s="79" t="s">
-        <v>131</v>
-      </c>
-      <c r="M51" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="N51" s="80"/>
-      <c r="O51" s="80" t="s">
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="79"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="80" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="76"/>
-      <c r="B52" s="0" t="s">
+      <c r="M56" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="N56" s="81"/>
+      <c r="O56" s="81" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="77"/>
+      <c r="B57" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="81"/>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="81"/>
-      <c r="G52" s="81"/>
-      <c r="H52" s="81"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="81"/>
-      <c r="K52" s="81"/>
-      <c r="L52" s="82" t="s">
-        <v>134</v>
-      </c>
-      <c r="M52" s="82" t="s">
-        <v>135</v>
-      </c>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83" t="s">
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="82"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="83" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="76"/>
-      <c r="B53" s="0" t="s">
+      <c r="M57" s="83" t="s">
+        <v>137</v>
+      </c>
+      <c r="N57" s="84"/>
+      <c r="O57" s="84" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="77"/>
+      <c r="B58" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="81"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="81"/>
-      <c r="G53" s="81"/>
-      <c r="H53" s="81"/>
-      <c r="I53" s="81"/>
-      <c r="J53" s="81"/>
-      <c r="K53" s="81"/>
-      <c r="L53" s="82" t="s">
-        <v>137</v>
-      </c>
-      <c r="M53" s="82" t="s">
-        <v>138</v>
-      </c>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83" t="s">
+      <c r="C58" s="82"/>
+      <c r="D58" s="82"/>
+      <c r="E58" s="82"/>
+      <c r="F58" s="82"/>
+      <c r="G58" s="82"/>
+      <c r="H58" s="82"/>
+      <c r="I58" s="82"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="82"/>
+      <c r="L58" s="83" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="54" s="89" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="76"/>
-      <c r="B54" s="84" t="s">
+      <c r="M58" s="83" t="s">
+        <v>140</v>
+      </c>
+      <c r="N58" s="84"/>
+      <c r="O58" s="84" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" s="90" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="77"/>
+      <c r="B59" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="86" t="n">
+      <c r="C59" s="86"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="86"/>
+      <c r="G59" s="86"/>
+      <c r="H59" s="86"/>
+      <c r="I59" s="86"/>
+      <c r="J59" s="86"/>
+      <c r="K59" s="86"/>
+      <c r="L59" s="87" t="n">
         <v>6.51</v>
       </c>
-      <c r="M54" s="87" t="n">
+      <c r="M59" s="88" t="n">
         <v>6.27</v>
       </c>
-      <c r="N54" s="88"/>
-      <c r="O54" s="87" t="n">
+      <c r="N59" s="89"/>
+      <c r="O59" s="88" t="n">
         <v>7.71</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="70" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78" t="n">
+      <c r="B60" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="79"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="79"/>
+      <c r="F60" s="79" t="n">
         <v>96.4</v>
       </c>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="78"/>
-      <c r="K55" s="78" t="n">
+      <c r="G60" s="79"/>
+      <c r="H60" s="79"/>
+      <c r="I60" s="79"/>
+      <c r="J60" s="79"/>
+      <c r="K60" s="79" t="n">
         <v>83.6</v>
       </c>
-      <c r="L55" s="78"/>
-      <c r="M55" s="78"/>
-      <c r="N55" s="80"/>
-      <c r="O55" s="80"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="70"/>
-      <c r="B56" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="90" t="n">
+      <c r="L60" s="79"/>
+      <c r="M60" s="79"/>
+      <c r="N60" s="81"/>
+      <c r="O60" s="81"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="71"/>
+      <c r="B61" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
+      <c r="F61" s="91" t="n">
         <v>97.2</v>
       </c>
-      <c r="G56" s="81"/>
-      <c r="H56" s="81"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="81"/>
-      <c r="K56" s="81" t="n">
+      <c r="G61" s="82"/>
+      <c r="H61" s="82"/>
+      <c r="I61" s="82"/>
+      <c r="J61" s="82"/>
+      <c r="K61" s="82" t="n">
         <v>84.4</v>
       </c>
-      <c r="L56" s="83"/>
-      <c r="M56" s="83"/>
-      <c r="N56" s="83"/>
-      <c r="O56" s="83"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="70"/>
-      <c r="B57" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" s="85"/>
-      <c r="D57" s="85"/>
-      <c r="E57" s="85"/>
-      <c r="F57" s="85" t="n">
+      <c r="L61" s="84"/>
+      <c r="M61" s="84"/>
+      <c r="N61" s="84"/>
+      <c r="O61" s="84"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="71"/>
+      <c r="B62" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86" t="n">
         <v>95.6</v>
       </c>
-      <c r="G57" s="85"/>
-      <c r="H57" s="85"/>
-      <c r="I57" s="85"/>
-      <c r="J57" s="85"/>
-      <c r="K57" s="87" t="n">
+      <c r="G62" s="86"/>
+      <c r="H62" s="86"/>
+      <c r="I62" s="86"/>
+      <c r="J62" s="86"/>
+      <c r="K62" s="88" t="n">
         <v>85.1</v>
       </c>
-      <c r="L57" s="88"/>
-      <c r="M57" s="88"/>
-      <c r="N57" s="88"/>
-      <c r="O57" s="88"/>
-    </row>
-    <row r="58" s="98" customFormat="true" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="91" t="s">
+      <c r="L62" s="89"/>
+      <c r="M62" s="89"/>
+      <c r="N62" s="89"/>
+      <c r="O62" s="89"/>
+    </row>
+    <row r="63" s="99" customFormat="true" ht="27.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B58" s="92" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="93"/>
-      <c r="D58" s="94" t="n">
+      <c r="B63" s="93" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="94"/>
+      <c r="D63" s="95" t="n">
         <v>49.6</v>
       </c>
-      <c r="E58" s="95" t="n">
+      <c r="E63" s="96" t="n">
         <v>89.4</v>
       </c>
-      <c r="F58" s="93"/>
-      <c r="G58" s="95" t="n">
+      <c r="F63" s="94"/>
+      <c r="G63" s="96" t="n">
         <v>88.2</v>
       </c>
-      <c r="H58" s="96" t="n">
+      <c r="H63" s="97" t="n">
         <v>93.9</v>
       </c>
-      <c r="I58" s="93"/>
-      <c r="J58" s="93"/>
-      <c r="K58" s="97"/>
-      <c r="L58" s="97"/>
-      <c r="M58" s="97"/>
-      <c r="N58" s="97"/>
-      <c r="O58" s="97"/>
-    </row>
-    <row r="59" s="97" customFormat="true" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="99" t="s">
+      <c r="I63" s="94"/>
+      <c r="J63" s="94"/>
+      <c r="K63" s="98"/>
+      <c r="L63" s="98"/>
+      <c r="M63" s="98"/>
+      <c r="N63" s="98"/>
+      <c r="O63" s="98"/>
+    </row>
+    <row r="64" s="98" customFormat="true" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B59" s="100" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
-      <c r="F59" s="93"/>
-      <c r="G59" s="93"/>
-      <c r="H59" s="93"/>
-      <c r="I59" s="93"/>
-      <c r="J59" s="93"/>
-      <c r="L59" s="101" t="s">
-        <v>145</v>
-      </c>
-      <c r="M59" s="101" t="s">
-        <v>145</v>
-      </c>
-      <c r="O59" s="101" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B64" s="101" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="94"/>
+      <c r="D64" s="94"/>
+      <c r="E64" s="94"/>
+      <c r="F64" s="94"/>
+      <c r="G64" s="94"/>
+      <c r="H64" s="94"/>
+      <c r="I64" s="94"/>
+      <c r="J64" s="94"/>
+      <c r="L64" s="102" t="s">
+        <v>147</v>
+      </c>
+      <c r="M64" s="102" t="s">
+        <v>147</v>
+      </c>
+      <c r="O64" s="102" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A1:C1"/>
@@ -2929,13 +3267,13 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H18:J18"/>
-    <mergeCell ref="C34:K34"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="C39:K39"/>
+    <mergeCell ref="L39:O39"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A60:A62"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="A Convolutional Neural Network for Modelling Sentences"/>
@@ -2961,8 +3299,9 @@
     <hyperlink ref="B27" r:id="rId21" display="Elec2"/>
     <hyperlink ref="B28" r:id="rId22" display="RCV1-multi"/>
     <hyperlink ref="B29" r:id="rId23" display="RCV1-single"/>
-    <hyperlink ref="G35" r:id="rId24" display="Sentiment140"/>
-    <hyperlink ref="M35" r:id="rId25" display="Elec2"/>
+    <hyperlink ref="B31" r:id="rId24" display="AG’s News"/>
+    <hyperlink ref="G40" r:id="rId25" display="Sentiment140"/>
+    <hyperlink ref="M40" r:id="rId26" display="Elec2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2981,18 +3320,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>146</v>
+      <c r="A1" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3004,4 +3343,251 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.6"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="94" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="103" width="11.4696356275304"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="94" width="75.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="98" width="65.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="98" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="104" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="105"/>
+    </row>
+    <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="94" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="106" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="104"/>
+      <c r="C3" s="94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="104"/>
+      <c r="C4" s="94" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="104" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="104"/>
+      <c r="C5" s="94" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="104" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="94" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" s="109" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="104" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+    </row>
+    <row r="8" s="109" customFormat="true" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="107"/>
+      <c r="B8" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+    </row>
+    <row r="9" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="107"/>
+    </row>
+    <row r="10" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="110" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="111"/>
+      <c r="B11" s="110" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="111"/>
+      <c r="B12" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="111" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="94" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="111"/>
+      <c r="B14" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="112" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="111"/>
+      <c r="B15" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="111" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="110" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="111"/>
+      <c r="B17" s="110" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="111"/>
+      <c r="B18" s="110" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="111" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="110" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="94" t="n">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="111"/>
+      <c r="B20" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="112" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="111"/>
+      <c r="B21" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="104" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="104"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="https://github.com/zhangxiangxiao/Crepe"/>
+    <hyperlink ref="C4" r:id="rId2" display="Xiang Zhang, et al. Character-level convolutional networks for text classification. NIPS 2015"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>